<commit_message>
Attempting to debug a classification issue. N12_L should be classified normal according to the visualization, but is returning abnormal elsewhere.
</commit_message>
<xml_diff>
--- a/Solution3/Results/Bootstrapping Results.xlsx
+++ b/Solution3/Results/Bootstrapping Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8112D4B0-145E-4616-911F-EC1FD27E24B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83635C65-5A39-4DFE-ABBE-5A1F7867B3C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19162,7 +19162,7 @@
   <dimension ref="A1:J1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="C2" sqref="C2:C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Organizes and makes changes to cv_analysis_svm (prints fpr and tpr now) and grad_cam_vis (runs viz for all images in one call)
</commit_message>
<xml_diff>
--- a/Solution3/Results/Bootstrapping Results.xlsx
+++ b/Solution3/Results/Bootstrapping Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83635C65-5A39-4DFE-ABBE-5A1F7867B3C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BDB9C3-8420-471F-BB15-1C07FF50A1F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="114">
   <si>
     <t>Image</t>
   </si>
@@ -283,54 +283,6 @@
     <t>AD9_R.png</t>
   </si>
   <si>
-    <t>AUC = 0.8434959349593496</t>
-  </si>
-  <si>
-    <t>AUC = 0.747096399535424</t>
-  </si>
-  <si>
-    <t>Avg AUC = 0.7453476112190803</t>
-  </si>
-  <si>
-    <t>Stdev AUC = 0.048833888137899954</t>
-  </si>
-  <si>
-    <t>Avg AUC = 0.8425508614484579</t>
-  </si>
-  <si>
-    <t>Stdev AUC = 0.04095131194617225</t>
-  </si>
-  <si>
-    <t>AUC = 0.8678861788617888</t>
-  </si>
-  <si>
-    <t>Avg AUC = 0.8657814418428518</t>
-  </si>
-  <si>
-    <t>Stdev AUC = 0.03788266071965637</t>
-  </si>
-  <si>
-    <t>AUC = 0.8437862950058073</t>
-  </si>
-  <si>
-    <t>Avg AUC = 0.8430019719881486</t>
-  </si>
-  <si>
-    <t>Stdev AUC = 0.03944443472042711</t>
-  </si>
-  <si>
-    <t>95% CI 0.7590011614401858 to 0.9146270396270396</t>
-  </si>
-  <si>
-    <t>95% CI 0.7866430260047281 to 0.9302325581395349</t>
-  </si>
-  <si>
-    <t>95% CI 0.6488372093023256 to 0.8375</t>
-  </si>
-  <si>
-    <t>95% CI 0.7663742690058479 to 0.9160859465737514</t>
-  </si>
-  <si>
     <t>Radiologist Prediction</t>
   </si>
   <si>
@@ -344,6 +296,75 @@
   </si>
   <si>
     <t>Machine Confidence Values</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>Radiologist</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>TPR</t>
+  </si>
+  <si>
+    <t>FPR</t>
+  </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <t>Stdev AUC = 0.04266975447398629</t>
+  </si>
+  <si>
+    <t>Avg AUC = 0.8694333861611719</t>
+  </si>
+  <si>
+    <t>95% CI 0.7779874213836478 to 0.9465737514518001</t>
+  </si>
+  <si>
+    <t>Machine+Radiologist</t>
+  </si>
+  <si>
+    <t>AUC = 0.8716608594657375</t>
+  </si>
+  <si>
+    <t>Avg AUC = 0.882803413772382</t>
+  </si>
+  <si>
+    <t>Stdev AUC = 0.03659941370481901</t>
+  </si>
+  <si>
+    <t>95% CI 0.8061414392059553 to 0.9459302325581395</t>
+  </si>
+  <si>
+    <t>AUC = 0.883855981416957</t>
+  </si>
+  <si>
+    <t>AUC = 0.8176538908246226</t>
+  </si>
+  <si>
+    <t>Avg AUC = 0.8157147301674192</t>
+  </si>
+  <si>
+    <t>Stdev AUC = 0.05099475071469199</t>
+  </si>
+  <si>
+    <t>95% CI 0.7148664343786294 to 0.9070847851335656</t>
+  </si>
+  <si>
+    <t>Avg AUC = 0.765463515480463</t>
+  </si>
+  <si>
+    <t>AUC = 0.7682926829268293</t>
+  </si>
+  <si>
+    <t>Stdev AUC = 0.05387715591742631</t>
+  </si>
+  <si>
+    <t>95% CI 0.6477541371158393 to 0.8589285714285714</t>
   </si>
 </sst>
 </file>
@@ -727,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1001"/>
+  <dimension ref="A1:P1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,10 +765,14 @@
     <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -755,25 +780,37 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="F1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="G1" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -789,17 +826,35 @@
       <c r="F2">
         <v>0.81158071168611701</v>
       </c>
+      <c r="G2">
+        <v>0.462857142</v>
+      </c>
       <c r="H2" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="I2">
         <v>0.75959302325581302</v>
       </c>
       <c r="J2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="L2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2">
+        <v>0.56626506024096301</v>
+      </c>
+      <c r="N2">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="O2">
+        <v>0.439024390243902</v>
+      </c>
+      <c r="P2">
+        <v>0.63066202090592305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -815,14 +870,32 @@
       <c r="F3">
         <v>4.5507566689372697E-2</v>
       </c>
+      <c r="G3">
+        <v>0.305714285999999</v>
+      </c>
       <c r="I3">
         <v>0.77113095238095197</v>
       </c>
       <c r="J3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="L3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M3">
+        <v>0.80722891566264998</v>
+      </c>
+      <c r="N3">
+        <v>0.69047619047619002</v>
+      </c>
+      <c r="O3">
+        <v>7.3170731707316999E-2</v>
+      </c>
+      <c r="P3">
+        <v>0.808652729384436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -838,14 +911,32 @@
       <c r="F4">
         <v>0.26762220056483899</v>
       </c>
+      <c r="G4">
+        <v>0.54666666600000002</v>
+      </c>
       <c r="I4">
         <v>0.72559523809523796</v>
       </c>
       <c r="J4" t="s">
+        <v>113</v>
+      </c>
+      <c r="L4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>0.74698795180722799</v>
+      </c>
+      <c r="N4">
+        <v>0.73809523809523803</v>
+      </c>
+      <c r="O4">
+        <v>0.24390243902438999</v>
+      </c>
+      <c r="P4">
+        <v>0.76829268292682895</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -861,11 +952,14 @@
       <c r="F5">
         <v>0.75254947086361201</v>
       </c>
+      <c r="G5">
+        <v>0.40571428599999898</v>
+      </c>
       <c r="I5">
         <v>0.69356725146198805</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -881,11 +975,14 @@
       <c r="F6">
         <v>0.82360418493219301</v>
       </c>
+      <c r="G6">
+        <v>0.182857142</v>
+      </c>
       <c r="I6">
         <v>0.70099255583126496</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -901,11 +998,14 @@
       <c r="F7">
         <v>0.68428237988162599</v>
       </c>
+      <c r="G7">
+        <v>0.44400000000000001</v>
+      </c>
       <c r="I7">
         <v>0.746428571428571</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -921,11 +1021,14 @@
       <c r="F8">
         <v>1.3264509721530799</v>
       </c>
+      <c r="G8">
+        <v>0.29857142799999897</v>
+      </c>
       <c r="I8">
         <v>0.75684523809523796</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -941,11 +1044,14 @@
       <c r="F9">
         <v>1.22008367281696</v>
       </c>
+      <c r="G9">
+        <v>0.55466666599999903</v>
+      </c>
       <c r="I9">
         <v>0.85436046511627906</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -961,11 +1067,14 @@
       <c r="F10">
         <v>0.93849857017257898</v>
       </c>
+      <c r="G10">
+        <v>0.32666666599999999</v>
+      </c>
       <c r="I10">
         <v>0.74796511627906903</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -981,11 +1090,14 @@
       <c r="F11">
         <v>9.2167647943307396E-2</v>
       </c>
+      <c r="G11">
+        <v>0.342857142</v>
+      </c>
       <c r="I11">
         <v>0.56725146198830401</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1001,11 +1113,14 @@
       <c r="F12">
         <v>0.41945976227049397</v>
       </c>
+      <c r="G12">
+        <v>6.6666665999999902E-2</v>
+      </c>
       <c r="I12">
         <v>0.72363636363636297</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1021,11 +1136,14 @@
       <c r="F13">
         <v>0.36910103774207298</v>
       </c>
+      <c r="G13">
+        <v>0.247692308</v>
+      </c>
       <c r="I13">
         <v>0.79529616724738605</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1041,11 +1159,14 @@
       <c r="F14">
         <v>3.7561201057496399E-2</v>
       </c>
+      <c r="G14">
+        <v>4.14285719999999E-2</v>
+      </c>
       <c r="I14">
         <v>0.73774509803921495</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1061,11 +1182,14 @@
       <c r="F15">
         <v>0.67944247649702205</v>
       </c>
+      <c r="G15">
+        <v>0.47538461599999998</v>
+      </c>
       <c r="I15">
         <v>0.65145348837209305</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1080,6 +1204,9 @@
       </c>
       <c r="F16">
         <v>0.84633490204838002</v>
+      </c>
+      <c r="G16">
+        <v>0.54933333399999995</v>
       </c>
       <c r="I16">
         <v>0.75029239766081801</v>
@@ -1101,6 +1228,9 @@
       <c r="F17">
         <v>0.25500476973991099</v>
       </c>
+      <c r="G17">
+        <v>8.4000000000000005E-2</v>
+      </c>
       <c r="I17">
         <v>0.73432055749128899</v>
       </c>
@@ -1121,6 +1251,9 @@
       <c r="F18">
         <v>0.138090099274774</v>
       </c>
+      <c r="G18">
+        <v>0.42399999999999999</v>
+      </c>
       <c r="I18">
         <v>0.72931442080378195</v>
       </c>
@@ -1141,6 +1274,9 @@
       <c r="F19">
         <v>0.38434609181177998</v>
       </c>
+      <c r="G19">
+        <v>0.347142858</v>
+      </c>
       <c r="I19">
         <v>0.69405594405594395</v>
       </c>
@@ -1161,6 +1297,9 @@
       <c r="F20">
         <v>0.57156958899549704</v>
       </c>
+      <c r="G20">
+        <v>0.61833333399999901</v>
+      </c>
       <c r="I20">
         <v>0.72122093023255796</v>
       </c>
@@ -1181,6 +1320,9 @@
       <c r="F21">
         <v>0.57236465546400295</v>
       </c>
+      <c r="G21">
+        <v>0.34153846199999999</v>
+      </c>
       <c r="I21">
         <v>0.78319623971797803</v>
       </c>
@@ -1201,6 +1343,9 @@
       <c r="F22">
         <v>0.32104359729568199</v>
       </c>
+      <c r="G22">
+        <v>0.37066666599999898</v>
+      </c>
       <c r="I22">
         <v>0.77010804321728599</v>
       </c>
@@ -1221,6 +1366,9 @@
       <c r="F23">
         <v>0.84744162113932897</v>
       </c>
+      <c r="G23">
+        <v>0.107999999999999</v>
+      </c>
       <c r="I23">
         <v>0.74622093023255798</v>
       </c>
@@ -1241,6 +1389,9 @@
       <c r="F24">
         <v>0.68428657548911598</v>
       </c>
+      <c r="G24">
+        <v>0.62714285800000003</v>
+      </c>
       <c r="I24">
         <v>0.708720930232558</v>
       </c>
@@ -1261,6 +1412,9 @@
       <c r="F25">
         <v>0.73870523761106099</v>
       </c>
+      <c r="G25">
+        <v>0.55333333399999896</v>
+      </c>
       <c r="I25">
         <v>0.79622093023255802</v>
       </c>
@@ -1281,6 +1435,9 @@
       <c r="F26">
         <v>0.82972840223759103</v>
       </c>
+      <c r="G26">
+        <v>0.37230769199999902</v>
+      </c>
       <c r="I26">
         <v>0.78284883720930198</v>
       </c>
@@ -1301,6 +1458,9 @@
       <c r="F27">
         <v>0.159837520161592</v>
       </c>
+      <c r="G27">
+        <v>0.104</v>
+      </c>
       <c r="I27">
         <v>0.65321637426900503</v>
       </c>
@@ -1321,6 +1481,9 @@
       <c r="F28">
         <v>0.33356481912192398</v>
       </c>
+      <c r="G28">
+        <v>0.24153846200000001</v>
+      </c>
       <c r="I28">
         <v>0.74320330969267101</v>
       </c>
@@ -1341,6 +1504,9 @@
       <c r="F29">
         <v>1.8022110465806E-3</v>
       </c>
+      <c r="G29">
+        <v>0.31733333399999902</v>
+      </c>
       <c r="I29">
         <v>0.71138211382113803</v>
       </c>
@@ -1361,6 +1527,9 @@
       <c r="F30">
         <v>0.16905871900786801</v>
       </c>
+      <c r="G30">
+        <v>0.59599999999999997</v>
+      </c>
       <c r="I30">
         <v>0.86484848484848398</v>
       </c>
@@ -1381,6 +1550,9 @@
       <c r="F31">
         <v>8.4087474090243905E-2</v>
       </c>
+      <c r="G31">
+        <v>0.62142857200000001</v>
+      </c>
       <c r="I31">
         <v>0.72296511627906901</v>
       </c>
@@ -1401,6 +1573,9 @@
       <c r="F32">
         <v>0.205389024712919</v>
       </c>
+      <c r="G32">
+        <v>0.157142858</v>
+      </c>
       <c r="I32">
         <v>0.73372093023255802</v>
       </c>
@@ -1421,6 +1596,9 @@
       <c r="F33">
         <v>2.3360445899143101E-2</v>
       </c>
+      <c r="G33">
+        <v>0.34399999999999997</v>
+      </c>
       <c r="I33">
         <v>0.75616921269095105</v>
       </c>
@@ -1441,6 +1619,9 @@
       <c r="F34">
         <v>0.228590067415471</v>
       </c>
+      <c r="G34">
+        <v>0.54533333399999995</v>
+      </c>
       <c r="I34">
         <v>0.73363636363636298</v>
       </c>
@@ -1461,6 +1642,9 @@
       <c r="F35">
         <v>0.42290305522835298</v>
       </c>
+      <c r="G35">
+        <v>0.62142857200000001</v>
+      </c>
       <c r="I35">
         <v>0.783625730994152</v>
       </c>
@@ -1481,6 +1665,9 @@
       <c r="F36">
         <v>7.3276186268897606E-2</v>
       </c>
+      <c r="G36">
+        <v>0.53857142799999902</v>
+      </c>
       <c r="I36">
         <v>0.80757931844888298</v>
       </c>
@@ -1501,6 +1688,9 @@
       <c r="F37">
         <v>0.30089055045213298</v>
       </c>
+      <c r="G37">
+        <v>0.49333333399999901</v>
+      </c>
       <c r="I37">
         <v>0.71286549707602298</v>
       </c>
@@ -1521,6 +1711,9 @@
       <c r="F38">
         <v>0.41630424262259402</v>
       </c>
+      <c r="G38">
+        <v>0.133333334</v>
+      </c>
       <c r="I38">
         <v>0.736662531017369</v>
       </c>
@@ -1541,6 +1734,9 @@
       <c r="F39">
         <v>0.92037222304330102</v>
       </c>
+      <c r="G39">
+        <v>0.40142857199999998</v>
+      </c>
       <c r="I39">
         <v>0.74679487179487103</v>
       </c>
@@ -1561,6 +1757,9 @@
       <c r="F40">
         <v>6.8521952635367797E-2</v>
       </c>
+      <c r="G40">
+        <v>0.55733333399999996</v>
+      </c>
       <c r="I40">
         <v>0.75813008130081205</v>
       </c>
@@ -1581,6 +1780,9 @@
       <c r="F41">
         <v>1.5502990199389699</v>
       </c>
+      <c r="G41">
+        <v>0.42307692400000002</v>
+      </c>
       <c r="I41">
         <v>0.83110465116278998</v>
       </c>
@@ -1601,6 +1803,9 @@
       <c r="F42">
         <v>1.18519122599903</v>
       </c>
+      <c r="G42">
+        <v>0.15428571399999899</v>
+      </c>
       <c r="I42">
         <v>0.72022332506203401</v>
       </c>
@@ -1621,6 +1826,9 @@
       <c r="F43">
         <v>0.116232855540533</v>
       </c>
+      <c r="G43">
+        <v>0.44571428599999902</v>
+      </c>
       <c r="I43">
         <v>0.74767711962833905</v>
       </c>
@@ -1641,6 +1849,9 @@
       <c r="F44">
         <v>1.87672190609281</v>
       </c>
+      <c r="G44">
+        <v>0.375384616</v>
+      </c>
       <c r="I44">
         <v>0.73906619385342798</v>
       </c>
@@ -1661,6 +1872,9 @@
       <c r="F45">
         <v>0.57385945128221505</v>
       </c>
+      <c r="G45">
+        <v>0.59285714199999995</v>
+      </c>
       <c r="I45">
         <v>0.78379953379953304</v>
       </c>
@@ -1681,6 +1895,9 @@
       <c r="F46">
         <v>1.03624389783241</v>
       </c>
+      <c r="G46">
+        <v>0.39571428599999903</v>
+      </c>
       <c r="I46">
         <v>0.75697674418604599</v>
       </c>
@@ -1701,6 +1918,9 @@
       <c r="F47">
         <v>0.22145864710528901</v>
       </c>
+      <c r="G47">
+        <v>0.56666666600000004</v>
+      </c>
       <c r="I47">
         <v>0.75730994152046704</v>
       </c>
@@ -1721,6 +1941,9 @@
       <c r="F48">
         <v>0.17354797615088</v>
       </c>
+      <c r="G48">
+        <v>0.29428571399999998</v>
+      </c>
       <c r="I48">
         <v>0.73461091753774599</v>
       </c>
@@ -1741,6 +1964,9 @@
       <c r="F49">
         <v>0.768006556332401</v>
       </c>
+      <c r="G49">
+        <v>0.14000000000000001</v>
+      </c>
       <c r="I49">
         <v>0.85340775558166804</v>
       </c>
@@ -1761,6 +1987,9 @@
       <c r="F50">
         <v>0.35823657261998199</v>
       </c>
+      <c r="G50">
+        <v>0.60666666599999997</v>
+      </c>
       <c r="I50">
         <v>0.77061556329849001</v>
       </c>
@@ -1781,6 +2010,9 @@
       <c r="F51">
         <v>0.35650303754665102</v>
       </c>
+      <c r="G51">
+        <v>0.18266666599999901</v>
+      </c>
       <c r="I51">
         <v>0.66308139534883703</v>
       </c>
@@ -1801,6 +2033,9 @@
       <c r="F52">
         <v>0.96990927169495</v>
       </c>
+      <c r="G52">
+        <v>2.9333333999999898E-2</v>
+      </c>
       <c r="I52">
         <v>0.72843822843822803</v>
       </c>
@@ -1821,6 +2056,9 @@
       <c r="F53">
         <v>0.1479791782762</v>
       </c>
+      <c r="G53">
+        <v>0.39714285799999999</v>
+      </c>
       <c r="I53">
         <v>0.77034883720930203</v>
       </c>
@@ -1841,6 +2079,9 @@
       <c r="F54">
         <v>0.69492906458870496</v>
       </c>
+      <c r="G54">
+        <v>0.62428571399999999</v>
+      </c>
       <c r="I54">
         <v>0.72125435540069605</v>
       </c>
@@ -1861,6 +2102,9 @@
       <c r="F55">
         <v>0.60149786394403604</v>
       </c>
+      <c r="G55">
+        <v>0.42249999999999999</v>
+      </c>
       <c r="I55">
         <v>0.78110465116279004</v>
       </c>
@@ -1881,6 +2125,9 @@
       <c r="F56">
         <v>0.248330090544158</v>
       </c>
+      <c r="G56">
+        <v>2.1333333999999898E-2</v>
+      </c>
       <c r="I56">
         <v>0.646220930232558</v>
       </c>
@@ -1901,6 +2148,9 @@
       <c r="F57">
         <v>0.91185392753868499</v>
       </c>
+      <c r="G57">
+        <v>0.22</v>
+      </c>
       <c r="I57">
         <v>0.75709219858155996</v>
       </c>
@@ -1921,6 +2171,9 @@
       <c r="F58">
         <v>0.43911827709926199</v>
       </c>
+      <c r="G58">
+        <v>0.16666666599999999</v>
+      </c>
       <c r="I58">
         <v>0.74265569917743801</v>
       </c>
@@ -1941,6 +2194,9 @@
       <c r="F59">
         <v>2.26797417528001E-2</v>
       </c>
+      <c r="G59">
+        <v>0.71599999999999997</v>
+      </c>
       <c r="I59">
         <v>0.68450292397660795</v>
       </c>
@@ -1961,6 +2217,9 @@
       <c r="F60">
         <v>0.13831317259753201</v>
       </c>
+      <c r="G60">
+        <v>0.28923077000000003</v>
+      </c>
       <c r="I60">
         <v>0.76339285714285698</v>
       </c>
@@ -1981,6 +2240,9 @@
       <c r="F61">
         <v>0.47042617466639702</v>
       </c>
+      <c r="G61">
+        <v>4.6153839999999403E-3</v>
+      </c>
       <c r="I61">
         <v>0.818448883666275</v>
       </c>
@@ -2001,6 +2263,9 @@
       <c r="F62">
         <v>1.01373630242322</v>
       </c>
+      <c r="G62">
+        <v>0.70799999999999996</v>
+      </c>
       <c r="I62">
         <v>0.83011695906432703</v>
       </c>
@@ -2021,6 +2286,9 @@
       <c r="F63">
         <v>1.5865646177950601</v>
       </c>
+      <c r="G63">
+        <v>0.08</v>
+      </c>
       <c r="I63">
         <v>0.7232868757259</v>
       </c>
@@ -2041,6 +2309,9 @@
       <c r="F64">
         <v>0.38698091237340998</v>
       </c>
+      <c r="G64">
+        <v>0.20533333400000001</v>
+      </c>
       <c r="I64">
         <v>0.79186046511627906</v>
       </c>
@@ -2061,6 +2332,9 @@
       <c r="F65">
         <v>0.59639900584343297</v>
       </c>
+      <c r="G65">
+        <v>0.342857142</v>
+      </c>
       <c r="I65">
         <v>0.74529964747356003</v>
       </c>
@@ -2081,6 +2355,9 @@
       <c r="F66">
         <v>0.20977882930898301</v>
       </c>
+      <c r="G66">
+        <v>0.27428571399999901</v>
+      </c>
       <c r="I66">
         <v>0.75935672514619801</v>
       </c>
@@ -2101,6 +2378,9 @@
       <c r="F67">
         <v>0.19299193835827499</v>
       </c>
+      <c r="G67">
+        <v>0.65428571400000002</v>
+      </c>
       <c r="I67">
         <v>0.71004700352526395</v>
       </c>
@@ -2121,6 +2401,9 @@
       <c r="F68">
         <v>0.285014747006889</v>
       </c>
+      <c r="G68">
+        <v>0.51200000000000001</v>
+      </c>
       <c r="I68">
         <v>0.84736842105263099</v>
       </c>
@@ -2141,6 +2424,9 @@
       <c r="F69">
         <v>0.58157271093767404</v>
       </c>
+      <c r="G69">
+        <v>0.22769230800000001</v>
+      </c>
       <c r="I69">
         <v>0.68699186991869898</v>
       </c>
@@ -2161,6 +2447,9 @@
       <c r="F70">
         <v>1.4550834802389701</v>
       </c>
+      <c r="G70">
+        <v>0.57428571399999995</v>
+      </c>
       <c r="I70">
         <v>0.75472813238770597</v>
       </c>
@@ -2181,6 +2470,9 @@
       <c r="F71">
         <v>0.225915484774173</v>
       </c>
+      <c r="G71">
+        <v>0.745714286</v>
+      </c>
       <c r="I71">
         <v>0.761072261072261</v>
       </c>
@@ -2201,6 +2493,9 @@
       <c r="F72">
         <v>0.55960496622880496</v>
       </c>
+      <c r="G72">
+        <v>0.14000000000000001</v>
+      </c>
       <c r="I72">
         <v>0.73459302325581399</v>
       </c>
@@ -2221,6 +2516,9 @@
       <c r="F73">
         <v>0.54368533437423405</v>
       </c>
+      <c r="G73">
+        <v>0.42266666600000002</v>
+      </c>
       <c r="I73">
         <v>0.77383720930232502</v>
       </c>
@@ -2241,6 +2539,9 @@
       <c r="F74">
         <v>0.18228494773872</v>
       </c>
+      <c r="G74">
+        <v>0.30249999999999999</v>
+      </c>
       <c r="I74">
         <v>0.81542617046818699</v>
       </c>
@@ -2261,6 +2562,9 @@
       <c r="F75">
         <v>0.22409603330090599</v>
       </c>
+      <c r="G75">
+        <v>0.06</v>
+      </c>
       <c r="I75">
         <v>0.780552291421856</v>
       </c>
@@ -2281,6 +2585,9 @@
       <c r="F76">
         <v>1.0042629465845201</v>
       </c>
+      <c r="G76">
+        <v>4.8571428E-2</v>
+      </c>
       <c r="I76">
         <v>0.72122093023255796</v>
       </c>
@@ -2301,6 +2608,9 @@
       <c r="F77">
         <v>0.39898207214854198</v>
       </c>
+      <c r="G77">
+        <v>0.27</v>
+      </c>
       <c r="I77">
         <v>0.875440658049353</v>
       </c>
@@ -2321,6 +2631,9 @@
       <c r="F78">
         <v>0.39680196072851098</v>
       </c>
+      <c r="G78">
+        <v>0.13866666599999999</v>
+      </c>
       <c r="I78">
         <v>0.75684523809523796</v>
       </c>
@@ -2341,6 +2654,9 @@
       <c r="F79">
         <v>0.95548600231391201</v>
       </c>
+      <c r="G79">
+        <v>0.152307691999999</v>
+      </c>
       <c r="I79">
         <v>0.65614035087719302</v>
       </c>
@@ -2361,6 +2677,9 @@
       <c r="F80">
         <v>0.45386297580691698</v>
       </c>
+      <c r="G80">
+        <v>0.13285714200000001</v>
+      </c>
       <c r="I80">
         <v>0.72649823736780195</v>
       </c>
@@ -2381,6 +2700,9 @@
       <c r="F81">
         <v>0.78720394537391503</v>
       </c>
+      <c r="G81">
+        <v>0.48285714200000002</v>
+      </c>
       <c r="I81">
         <v>0.73688811188811099</v>
       </c>
@@ -2401,6 +2723,9 @@
       <c r="F82">
         <v>0.47837338522323097</v>
       </c>
+      <c r="G82">
+        <v>0.118666666</v>
+      </c>
       <c r="I82">
         <v>0.67508710801393701</v>
       </c>
@@ -2421,6 +2746,9 @@
       <c r="F83">
         <v>0.30997447369823999</v>
       </c>
+      <c r="G83">
+        <v>5.5999999999999897E-2</v>
+      </c>
       <c r="I83">
         <v>0.72363636363636297</v>
       </c>
@@ -2440,6 +2768,9 @@
       </c>
       <c r="F84">
         <v>0.64216414026244295</v>
+      </c>
+      <c r="G84">
+        <v>0.21714285799999999</v>
       </c>
       <c r="I84">
         <v>0.73099415204678297</v>
@@ -7037,10 +7368,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC718A7F-4416-4837-9CBF-C11F5F01DF1B}">
-  <dimension ref="A1:J1001"/>
+  <dimension ref="A1:P1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7055,9 +7386,11 @@
     <col min="8" max="8" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7065,286 +7398,433 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="F1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="G1" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
         <v>0.84976750908409004</v>
       </c>
+      <c r="G2">
+        <v>0.462857142</v>
+      </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="I2">
         <v>0.86860465116278995</v>
       </c>
       <c r="J2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="L2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2">
+        <v>0.65060240963855398</v>
+      </c>
+      <c r="N2">
+        <v>0.69047619047619002</v>
+      </c>
+      <c r="O2">
+        <v>0.39024390243902402</v>
+      </c>
+      <c r="P2">
+        <v>0.70789779326364699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
         <v>0.122918857778317</v>
       </c>
+      <c r="G3">
+        <v>0.305714285999999</v>
+      </c>
       <c r="I3">
         <v>0.862202380952381</v>
       </c>
       <c r="J3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="L3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M3">
+        <v>0.80722891566264998</v>
+      </c>
+      <c r="N3">
+        <v>0.69047619047619002</v>
+      </c>
+      <c r="O3">
+        <v>7.3170731707316999E-2</v>
+      </c>
+      <c r="P3">
+        <v>0.808652729384436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
         <v>0.32600277111027698</v>
       </c>
+      <c r="G4">
+        <v>0.54666666600000002</v>
+      </c>
       <c r="I4">
         <v>0.78928571428571404</v>
       </c>
       <c r="J4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="L4" t="s">
+        <v>100</v>
+      </c>
+      <c r="M4">
+        <v>0.843373493975903</v>
+      </c>
+      <c r="N4">
+        <v>0.80952380952380898</v>
+      </c>
+      <c r="O4">
+        <v>0.12195121951219499</v>
+      </c>
+      <c r="P4">
+        <v>0.81765389082462203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
         <v>7.4718752425197404E-2</v>
       </c>
+      <c r="G5">
+        <v>0.40571428599999898</v>
+      </c>
       <c r="I5">
         <v>0.76637426900584704</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <v>1.1275291118208</v>
       </c>
+      <c r="G6">
+        <v>0.182857142</v>
+      </c>
       <c r="I6">
         <v>0.83281637717121504</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
         <v>0.13437624729011199</v>
       </c>
+      <c r="G7">
+        <v>0.44400000000000001</v>
+      </c>
       <c r="I7">
         <v>0.85446428571428501</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
         <v>1.05502064744295</v>
       </c>
+      <c r="G8">
+        <v>0.29857142799999897</v>
+      </c>
       <c r="I8">
         <v>0.81785714285714195</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
         <v>0.83857755745559004</v>
       </c>
+      <c r="G9">
+        <v>0.55466666599999903</v>
+      </c>
       <c r="I9">
         <v>0.90436046511627899</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
         <v>0.72887397805778098</v>
       </c>
+      <c r="G10">
+        <v>0.32666666599999999</v>
+      </c>
       <c r="I10">
         <v>0.892732558139534</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
         <v>0.18823340825901</v>
       </c>
+      <c r="G11">
+        <v>0.342857142</v>
+      </c>
       <c r="I11">
         <v>0.73713450292397598</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
         <v>0.33638823372545901</v>
       </c>
+      <c r="G12">
+        <v>6.6666665999999902E-2</v>
+      </c>
       <c r="I12">
         <v>0.83393939393939298</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
         <v>0.31875912853645899</v>
       </c>
+      <c r="G13">
+        <v>0.247692308</v>
+      </c>
       <c r="I13">
         <v>0.85598141695702601</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
         <v>0.102505828040737</v>
       </c>
+      <c r="G14">
+        <v>4.14285719999999E-2</v>
+      </c>
       <c r="I14">
         <v>0.82965686274509798</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
         <v>0.44281322308027998</v>
       </c>
+      <c r="G15">
+        <v>0.47538461599999998</v>
+      </c>
       <c r="I15">
         <v>0.80872093023255798</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
         <v>1.04208934104532</v>
+      </c>
+      <c r="G16">
+        <v>0.54933333399999995</v>
       </c>
       <c r="I16">
         <v>0.85847953216374195</v>
@@ -7357,11 +7837,17 @@
       <c r="B17">
         <v>0</v>
       </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
         <v>0.19914109246025599</v>
+      </c>
+      <c r="G17">
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="I17">
         <v>0.81852497096399501</v>
@@ -7374,11 +7860,17 @@
       <c r="B18">
         <v>0</v>
       </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
         <v>0.42477133924489902</v>
+      </c>
+      <c r="G18">
+        <v>0.42399999999999999</v>
       </c>
       <c r="I18">
         <v>0.82092198581560205</v>
@@ -7391,11 +7883,17 @@
       <c r="B19">
         <v>0</v>
       </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
         <v>0.12519442658742</v>
+      </c>
+      <c r="G19">
+        <v>0.347142858</v>
       </c>
       <c r="I19">
         <v>0.82634032634032595</v>
@@ -7408,11 +7906,17 @@
       <c r="B20">
         <v>0</v>
       </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
         <v>0.82116669544785303</v>
+      </c>
+      <c r="G20">
+        <v>0.61833333399999901</v>
       </c>
       <c r="I20">
         <v>0.89011627906976698</v>
@@ -7425,11 +7929,17 @@
       <c r="B21">
         <v>0</v>
       </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21">
         <v>0.32905587232611999</v>
+      </c>
+      <c r="G21">
+        <v>0.34153846199999999</v>
       </c>
       <c r="I21">
         <v>0.905111633372502</v>
@@ -7442,11 +7952,17 @@
       <c r="B22">
         <v>0</v>
       </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22">
         <v>2.2167912924142399E-2</v>
+      </c>
+      <c r="G22">
+        <v>0.37066666599999898</v>
       </c>
       <c r="I22">
         <v>0.84603841536614599</v>
@@ -7459,11 +7975,17 @@
       <c r="B23">
         <v>0</v>
       </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
         <v>0.83087637096973499</v>
+      </c>
+      <c r="G23">
+        <v>0.107999999999999</v>
       </c>
       <c r="I23">
         <v>0.833720930232558</v>
@@ -7476,11 +7998,17 @@
       <c r="B24">
         <v>0</v>
       </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24">
         <v>0.93582873911394704</v>
+      </c>
+      <c r="G24">
+        <v>0.62714285800000003</v>
       </c>
       <c r="I24">
         <v>0.85174418604651103</v>
@@ -7493,11 +8021,17 @@
       <c r="B25">
         <v>0</v>
       </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
         <v>0.690435231939455</v>
+      </c>
+      <c r="G25">
+        <v>0.55333333399999896</v>
       </c>
       <c r="I25">
         <v>0.82209302325581401</v>
@@ -7510,11 +8044,17 @@
       <c r="B26">
         <v>0</v>
       </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26">
         <v>0.70537521386537205</v>
+      </c>
+      <c r="G26">
+        <v>0.37230769199999902</v>
       </c>
       <c r="I26">
         <v>0.85436046511627906</v>
@@ -7527,11 +8067,17 @@
       <c r="B27">
         <v>0</v>
       </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
         <v>6.1440556903876203E-2</v>
+      </c>
+      <c r="G27">
+        <v>0.104</v>
       </c>
       <c r="I27">
         <v>0.78157894736842104</v>
@@ -7544,11 +8090,17 @@
       <c r="B28">
         <v>0</v>
       </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
         <v>0.34489418232073499</v>
+      </c>
+      <c r="G28">
+        <v>0.24153846200000001</v>
       </c>
       <c r="I28">
         <v>0.84869976359337995</v>
@@ -7561,11 +8113,17 @@
       <c r="B29">
         <v>0</v>
       </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
         <v>5.2322103517424903E-2</v>
+      </c>
+      <c r="G29">
+        <v>0.31733333399999902</v>
       </c>
       <c r="I29">
         <v>0.85598141695702601</v>
@@ -7578,11 +8136,17 @@
       <c r="B30">
         <v>0</v>
       </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
         <v>0.26789703398014197</v>
+      </c>
+      <c r="G30">
+        <v>0.59599999999999997</v>
       </c>
       <c r="I30">
         <v>0.88454545454545397</v>
@@ -7595,11 +8159,17 @@
       <c r="B31">
         <v>0</v>
       </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
         <v>4.8867927562697602E-2</v>
+      </c>
+      <c r="G31">
+        <v>0.62142857200000001</v>
       </c>
       <c r="I31">
         <v>0.80872093023255798</v>
@@ -7612,11 +8182,17 @@
       <c r="B32">
         <v>0</v>
       </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
         <v>0.75990041190651703</v>
+      </c>
+      <c r="G32">
+        <v>0.157142858</v>
       </c>
       <c r="I32">
         <v>0.830232558139534</v>
@@ -7629,11 +8205,17 @@
       <c r="B33">
         <v>0</v>
       </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
         <v>0.108625597209939</v>
+      </c>
+      <c r="G33">
+        <v>0.34399999999999997</v>
       </c>
       <c r="I33">
         <v>0.88072855464159805</v>
@@ -7646,11 +8228,17 @@
       <c r="B34">
         <v>0</v>
       </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
         <v>0.116455544321481</v>
+      </c>
+      <c r="G34">
+        <v>0.54533333399999995</v>
       </c>
       <c r="I34">
         <v>0.83454545454545404</v>
@@ -7663,11 +8251,17 @@
       <c r="B35">
         <v>0</v>
       </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35">
         <v>0.117330757004213</v>
+      </c>
+      <c r="G35">
+        <v>0.62142857200000001</v>
       </c>
       <c r="I35">
         <v>0.90497076023391798</v>
@@ -7680,11 +8274,17 @@
       <c r="B36">
         <v>0</v>
       </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
         <v>9.0581173773334495E-2</v>
+      </c>
+      <c r="G36">
+        <v>0.53857142799999902</v>
       </c>
       <c r="I36">
         <v>0.86192714453583996</v>
@@ -7697,11 +8297,17 @@
       <c r="B37">
         <v>0</v>
       </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37">
         <v>0.86710398495736396</v>
+      </c>
+      <c r="G37">
+        <v>0.49333333399999901</v>
       </c>
       <c r="I37">
         <v>0.85350877192982399</v>
@@ -7714,11 +8320,17 @@
       <c r="B38">
         <v>0</v>
       </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38">
         <v>0.25259582970063699</v>
+      </c>
+      <c r="G38">
+        <v>0.133333334</v>
       </c>
       <c r="I38">
         <v>0.82009925558312602</v>
@@ -7731,11 +8343,17 @@
       <c r="B39">
         <v>0</v>
       </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="F39">
         <v>0.62760467913761497</v>
+      </c>
+      <c r="G39">
+        <v>0.40142857199999998</v>
       </c>
       <c r="I39">
         <v>0.84498834498834496</v>
@@ -7748,11 +8366,17 @@
       <c r="B40">
         <v>0</v>
       </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
         <v>0.36287913919054299</v>
+      </c>
+      <c r="G40">
+        <v>0.55733333399999996</v>
       </c>
       <c r="I40">
         <v>0.85569105691056901</v>
@@ -7765,11 +8389,17 @@
       <c r="B41">
         <v>0</v>
       </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41">
         <v>1.3251930398151299</v>
+      </c>
+      <c r="G41">
+        <v>0.42307692400000002</v>
       </c>
       <c r="I41">
         <v>0.92674418604651099</v>
@@ -7782,11 +8412,17 @@
       <c r="B42">
         <v>0</v>
       </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
         <v>1.6204337440597301</v>
+      </c>
+      <c r="G42">
+        <v>0.15428571399999899</v>
       </c>
       <c r="I42">
         <v>0.82971464019851104</v>
@@ -7799,11 +8435,17 @@
       <c r="B43">
         <v>1</v>
       </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
       <c r="E43">
         <v>1</v>
       </c>
       <c r="F43">
         <v>0.480323942187941</v>
+      </c>
+      <c r="G43">
+        <v>0.44571428599999902</v>
       </c>
       <c r="I43">
         <v>0.88008130081300795</v>
@@ -7816,11 +8458,17 @@
       <c r="B44">
         <v>1</v>
       </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="F44">
         <v>1.46712499055928</v>
+      </c>
+      <c r="G44">
+        <v>0.375384616</v>
       </c>
       <c r="I44">
         <v>0.87972813238770597</v>
@@ -7833,11 +8481,17 @@
       <c r="B45">
         <v>1</v>
       </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="F45">
         <v>0.96171576088197896</v>
+      </c>
+      <c r="G45">
+        <v>0.59285714199999995</v>
       </c>
       <c r="I45">
         <v>0.91462703962703895</v>
@@ -7850,11 +8504,17 @@
       <c r="B46">
         <v>1</v>
       </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
       <c r="E46">
         <v>1</v>
       </c>
       <c r="F46">
         <v>1.2782684923408201</v>
+      </c>
+      <c r="G46">
+        <v>0.39571428599999903</v>
       </c>
       <c r="I46">
         <v>0.82936046511627903</v>
@@ -7867,11 +8527,17 @@
       <c r="B47">
         <v>1</v>
       </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
       <c r="E47">
         <v>1</v>
       </c>
       <c r="F47">
         <v>6.8151988953702794E-2</v>
+      </c>
+      <c r="G47">
+        <v>0.56666666600000004</v>
       </c>
       <c r="I47">
         <v>0.85643274853801099</v>
@@ -7884,11 +8550,17 @@
       <c r="B48">
         <v>1</v>
       </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
       <c r="E48">
         <v>1</v>
       </c>
       <c r="F48">
         <v>0.82790220044294605</v>
+      </c>
+      <c r="G48">
+        <v>0.29428571399999998</v>
       </c>
       <c r="I48">
         <v>0.89169570267131204</v>
@@ -7901,11 +8573,17 @@
       <c r="B49">
         <v>1</v>
       </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49">
         <v>0.80206656268015797</v>
+      </c>
+      <c r="G49">
+        <v>0.14000000000000001</v>
       </c>
       <c r="I49">
         <v>0.91039952996474705</v>
@@ -7918,11 +8596,17 @@
       <c r="B50">
         <v>1</v>
       </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
       <c r="E50">
         <v>1</v>
       </c>
       <c r="F50">
         <v>0.42377600846545799</v>
+      </c>
+      <c r="G50">
+        <v>0.60666666599999997</v>
       </c>
       <c r="I50">
         <v>0.90331010452961602</v>
@@ -7935,11 +8619,17 @@
       <c r="B51">
         <v>1</v>
       </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
       <c r="E51">
         <v>1</v>
       </c>
       <c r="F51">
         <v>0.430031159173281</v>
+      </c>
+      <c r="G51">
+        <v>0.18266666599999901</v>
       </c>
       <c r="I51">
         <v>0.85784883720930205</v>
@@ -7952,11 +8642,17 @@
       <c r="B52">
         <v>1</v>
       </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
       <c r="E52">
         <v>1</v>
       </c>
       <c r="F52">
         <v>1.1302107525618299</v>
+      </c>
+      <c r="G52">
+        <v>2.9333333999999898E-2</v>
       </c>
       <c r="I52">
         <v>0.79370629370629298</v>
@@ -7969,11 +8665,17 @@
       <c r="B53">
         <v>1</v>
       </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
       <c r="E53">
         <v>1</v>
       </c>
       <c r="F53">
         <v>0.247439394073944</v>
+      </c>
+      <c r="G53">
+        <v>0.39714285799999999</v>
       </c>
       <c r="I53">
         <v>0.87936046511627897</v>
@@ -7986,11 +8688,17 @@
       <c r="B54">
         <v>1</v>
       </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
       <c r="E54">
         <v>1</v>
       </c>
       <c r="F54">
         <v>0.13325796433322801</v>
+      </c>
+      <c r="G54">
+        <v>0.62428571399999999</v>
       </c>
       <c r="I54">
         <v>0.86643437862950001</v>
@@ -8003,11 +8711,17 @@
       <c r="B55">
         <v>1</v>
       </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
       <c r="E55">
         <v>1</v>
       </c>
       <c r="F55">
         <v>0.784972499590046</v>
+      </c>
+      <c r="G55">
+        <v>0.42249999999999999</v>
       </c>
       <c r="I55">
         <v>0.82936046511627903</v>
@@ -8020,11 +8734,17 @@
       <c r="B56">
         <v>1</v>
       </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
       <c r="E56">
         <v>0</v>
       </c>
       <c r="F56">
         <v>0.53690058393024598</v>
+      </c>
+      <c r="G56">
+        <v>2.1333333999999898E-2</v>
       </c>
       <c r="I56">
         <v>0.80174418604651099</v>
@@ -8037,11 +8757,17 @@
       <c r="B57">
         <v>1</v>
       </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
       <c r="E57">
         <v>1</v>
       </c>
       <c r="F57">
         <v>0.75791189370758905</v>
+      </c>
+      <c r="G57">
+        <v>0.22</v>
       </c>
       <c r="I57">
         <v>0.86258865248226901</v>
@@ -8054,11 +8780,17 @@
       <c r="B58">
         <v>1</v>
       </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
       <c r="E58">
         <v>0</v>
       </c>
       <c r="F58">
         <v>0.13699888173408101</v>
+      </c>
+      <c r="G58">
+        <v>0.16666666599999999</v>
       </c>
       <c r="I58">
         <v>0.81316098707402995</v>
@@ -8071,11 +8803,17 @@
       <c r="B59">
         <v>1</v>
       </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
       <c r="E59">
         <v>1</v>
       </c>
       <c r="F59">
         <v>0.28705543893571001</v>
+      </c>
+      <c r="G59">
+        <v>0.71599999999999997</v>
       </c>
       <c r="I59">
         <v>0.77543859649122804</v>
@@ -8088,11 +8826,17 @@
       <c r="B60">
         <v>1</v>
       </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
       <c r="E60">
         <v>1</v>
       </c>
       <c r="F60">
         <v>8.7623437130377197E-3</v>
+      </c>
+      <c r="G60">
+        <v>0.28923077000000003</v>
       </c>
       <c r="I60">
         <v>0.88690476190476097</v>
@@ -8105,11 +8849,17 @@
       <c r="B61">
         <v>1</v>
       </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
       <c r="E61">
         <v>1</v>
       </c>
       <c r="F61">
         <v>0.13198327099673299</v>
+      </c>
+      <c r="G61">
+        <v>4.6153839999999403E-3</v>
       </c>
       <c r="I61">
         <v>0.88895417156286705</v>
@@ -8122,11 +8872,17 @@
       <c r="B62">
         <v>1</v>
       </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
       <c r="E62">
         <v>1</v>
       </c>
       <c r="F62">
         <v>0.92266404875613806</v>
+      </c>
+      <c r="G62">
+        <v>0.70799999999999996</v>
       </c>
       <c r="I62">
         <v>0.83713450292397595</v>
@@ -8139,11 +8895,17 @@
       <c r="B63">
         <v>1</v>
       </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
       <c r="E63">
         <v>1</v>
       </c>
       <c r="F63">
         <v>1.43129104587679</v>
+      </c>
+      <c r="G63">
+        <v>0.08</v>
       </c>
       <c r="I63">
         <v>0.83072009291521398</v>
@@ -8156,11 +8918,17 @@
       <c r="B64">
         <v>1</v>
       </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
       <c r="E64">
         <v>0</v>
       </c>
       <c r="F64">
         <v>1.25891263925061</v>
+      </c>
+      <c r="G64">
+        <v>0.20533333400000001</v>
       </c>
       <c r="I64">
         <v>0.91424418604651103</v>
@@ -8173,11 +8941,17 @@
       <c r="B65">
         <v>1</v>
       </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
       <c r="E65">
         <v>0</v>
       </c>
       <c r="F65">
         <v>0.41509770656081402</v>
+      </c>
+      <c r="G65">
+        <v>0.342857142</v>
       </c>
       <c r="I65">
         <v>0.83196239717978804</v>
@@ -8190,11 +8964,17 @@
       <c r="B66">
         <v>1</v>
       </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
       <c r="E66">
         <v>1</v>
       </c>
       <c r="F66">
         <v>0.303501756644948</v>
+      </c>
+      <c r="G66">
+        <v>0.27428571399999901</v>
       </c>
       <c r="I66">
         <v>0.792690058479532</v>
@@ -8207,11 +8987,17 @@
       <c r="B67">
         <v>1</v>
       </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
       <c r="E67">
         <v>1</v>
       </c>
       <c r="F67">
         <v>0.122756522876243</v>
+      </c>
+      <c r="G67">
+        <v>0.65428571400000002</v>
       </c>
       <c r="I67">
         <v>0.81286721504112802</v>
@@ -8224,11 +9010,17 @@
       <c r="B68">
         <v>1</v>
       </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
       <c r="E68">
         <v>1</v>
       </c>
       <c r="F68">
         <v>0.21995361128281399</v>
+      </c>
+      <c r="G68">
+        <v>0.51200000000000001</v>
       </c>
       <c r="I68">
         <v>0.90701754385964894</v>
@@ -8241,11 +9033,17 @@
       <c r="B69">
         <v>1</v>
       </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
       <c r="E69">
         <v>1</v>
       </c>
       <c r="F69">
         <v>0.52293670505767498</v>
+      </c>
+      <c r="G69">
+        <v>0.22769230800000001</v>
       </c>
       <c r="I69">
         <v>0.84378629500580704</v>
@@ -8258,11 +9056,17 @@
       <c r="B70">
         <v>1</v>
       </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
       <c r="E70">
         <v>1</v>
       </c>
       <c r="F70">
         <v>1.75890269818087</v>
+      </c>
+      <c r="G70">
+        <v>0.57428571399999995</v>
       </c>
       <c r="I70">
         <v>0.84544917257683205</v>
@@ -8275,11 +9079,17 @@
       <c r="B71">
         <v>1</v>
       </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
       <c r="E71">
         <v>1</v>
       </c>
       <c r="F71">
         <v>5.2612457111321502E-2</v>
+      </c>
+      <c r="G71">
+        <v>0.745714286</v>
       </c>
       <c r="I71">
         <v>0.84353146853146799</v>
@@ -8292,11 +9102,17 @@
       <c r="B72">
         <v>1</v>
       </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
       <c r="E72">
         <v>1</v>
       </c>
       <c r="F72">
         <v>0.41339679617501301</v>
+      </c>
+      <c r="G72">
+        <v>0.14000000000000001</v>
       </c>
       <c r="I72">
         <v>0.84273255813953396</v>
@@ -8309,11 +9125,17 @@
       <c r="B73">
         <v>1</v>
       </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
       <c r="E73">
         <v>1</v>
       </c>
       <c r="F73">
         <v>2.3477938579774101E-2</v>
+      </c>
+      <c r="G73">
+        <v>0.42266666600000002</v>
       </c>
       <c r="I73">
         <v>0.85959302325581299</v>
@@ -8326,11 +9148,17 @@
       <c r="B74">
         <v>1</v>
       </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
       <c r="E74">
         <v>1</v>
       </c>
       <c r="F74">
         <v>0.38622849625814598</v>
+      </c>
+      <c r="G74">
+        <v>0.30249999999999999</v>
       </c>
       <c r="I74">
         <v>0.91956782713085194</v>
@@ -8343,11 +9171,17 @@
       <c r="B75">
         <v>1</v>
       </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
       <c r="E75">
         <v>1</v>
       </c>
       <c r="F75">
         <v>0.67864491883398204</v>
+      </c>
+      <c r="G75">
+        <v>0.06</v>
       </c>
       <c r="I75">
         <v>0.88072855464159805</v>
@@ -8360,11 +9194,17 @@
       <c r="B76">
         <v>1</v>
       </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
       <c r="E76">
         <v>1</v>
       </c>
       <c r="F76">
         <v>0.96929746115308402</v>
+      </c>
+      <c r="G76">
+        <v>4.8571428E-2</v>
       </c>
       <c r="I76">
         <v>0.86598837209302304</v>
@@ -8377,11 +9217,17 @@
       <c r="B77">
         <v>1</v>
       </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
       <c r="E77">
         <v>1</v>
       </c>
       <c r="F77">
         <v>0.25506125216468001</v>
+      </c>
+      <c r="G77">
+        <v>0.27</v>
       </c>
       <c r="I77">
         <v>0.92685076380728504</v>
@@ -8394,11 +9240,17 @@
       <c r="B78">
         <v>1</v>
       </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
       <c r="E78">
         <v>1</v>
       </c>
       <c r="F78">
         <v>0.40465853783214401</v>
+      </c>
+      <c r="G78">
+        <v>0.13866666599999999</v>
       </c>
       <c r="I78">
         <v>0.79851190476190403</v>
@@ -8411,11 +9263,17 @@
       <c r="B79">
         <v>1</v>
       </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
       <c r="E79">
         <v>1</v>
       </c>
       <c r="F79">
         <v>0.52778822643479295</v>
+      </c>
+      <c r="G79">
+        <v>0.152307691999999</v>
       </c>
       <c r="I79">
         <v>0.777485380116959</v>
@@ -8428,11 +9286,17 @@
       <c r="B80">
         <v>1</v>
       </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
       <c r="E80">
         <v>1</v>
       </c>
       <c r="F80">
         <v>0.308437826398969</v>
+      </c>
+      <c r="G80">
+        <v>0.13285714200000001</v>
       </c>
       <c r="I80">
         <v>0.79435957696827197</v>
@@ -8445,11 +9309,17 @@
       <c r="B81">
         <v>1</v>
       </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
       <c r="E81">
         <v>0</v>
       </c>
       <c r="F81">
         <v>0.89434252594105001</v>
+      </c>
+      <c r="G81">
+        <v>0.48285714200000002</v>
       </c>
       <c r="I81">
         <v>0.77680652680652595</v>
@@ -8462,11 +9332,17 @@
       <c r="B82">
         <v>1</v>
       </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
       <c r="E82">
         <v>1</v>
       </c>
       <c r="F82">
         <v>1.1111824723253901E-2</v>
+      </c>
+      <c r="G82">
+        <v>0.118666666</v>
       </c>
       <c r="I82">
         <v>0.80807200929152101</v>
@@ -8479,11 +9355,17 @@
       <c r="B83">
         <v>1</v>
       </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
       <c r="E83">
         <v>1</v>
       </c>
       <c r="F83">
         <v>0.45796593972960298</v>
+      </c>
+      <c r="G83">
+        <v>5.5999999999999897E-2</v>
       </c>
       <c r="I83">
         <v>0.824242424242424</v>
@@ -8496,11 +9378,17 @@
       <c r="B84">
         <v>1</v>
       </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
       <c r="E84">
         <v>0</v>
       </c>
       <c r="F84">
         <v>0.494716803423709</v>
+      </c>
+      <c r="G84">
+        <v>0.21714285799999999</v>
       </c>
       <c r="I84">
         <v>0.85643274853801099</v>
@@ -13098,10 +13986,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD840D1-1D4B-4BA9-B0B8-24F9FD7C2C86}">
-  <dimension ref="A1:J1001"/>
+  <dimension ref="A1:P1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13116,9 +14004,11 @@
     <col min="8" max="8" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13126,286 +14016,433 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="F1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="G1" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
         <v>0.86214502534912196</v>
       </c>
+      <c r="G2">
+        <v>0.462857142</v>
+      </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="I2">
         <v>0.78284883720930198</v>
       </c>
       <c r="J2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="L2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2">
+        <v>0.67469879518072196</v>
+      </c>
+      <c r="N2">
+        <v>0.64285714285714202</v>
+      </c>
+      <c r="O2">
+        <v>0.292682926829268</v>
+      </c>
+      <c r="P2">
+        <v>0.77061556329849001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
         <v>0.116721912080721</v>
       </c>
+      <c r="G3">
+        <v>0.305714285999999</v>
+      </c>
       <c r="I3">
         <v>0.87261904761904696</v>
       </c>
       <c r="J3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="L3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M3">
+        <v>0.80722891566264998</v>
+      </c>
+      <c r="N3">
+        <v>0.69047619047619002</v>
+      </c>
+      <c r="O3">
+        <v>7.3170731707316999E-2</v>
+      </c>
+      <c r="P3">
+        <v>0.808652729384436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
         <v>0.56815072192228</v>
       </c>
+      <c r="G4">
+        <v>0.54666666600000002</v>
+      </c>
       <c r="I4">
         <v>0.78928571428571404</v>
       </c>
       <c r="J4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="L4" t="s">
+        <v>100</v>
+      </c>
+      <c r="M4">
+        <v>0.843373493975903</v>
+      </c>
+      <c r="N4">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="O4">
+        <v>0.146341463414634</v>
+      </c>
+      <c r="P4">
+        <v>0.88385598141695698</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
         <v>7.7045663940696799E-2</v>
       </c>
+      <c r="G5">
+        <v>0.40571428599999898</v>
+      </c>
       <c r="I5">
         <v>0.85029239766081799</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <v>0.78345625803863495</v>
       </c>
+      <c r="G6">
+        <v>0.182857142</v>
+      </c>
       <c r="I6">
         <v>0.86507444168734404</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
         <v>0.47036118483700701</v>
       </c>
+      <c r="G7">
+        <v>0.44400000000000001</v>
+      </c>
       <c r="I7">
         <v>0.81279761904761905</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
         <v>2.0921817748661602</v>
       </c>
+      <c r="G8">
+        <v>0.29857142799999897</v>
+      </c>
       <c r="I8">
         <v>0.80625000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
         <v>1.0556594289251799</v>
       </c>
+      <c r="G9">
+        <v>0.55466666599999903</v>
+      </c>
       <c r="I9">
         <v>0.878488372093023</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
         <v>1.0011940179323</v>
       </c>
+      <c r="G10">
+        <v>0.32666666599999999</v>
+      </c>
       <c r="I10">
         <v>0.82936046511627903</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
         <v>9.8604137987704801E-2</v>
       </c>
+      <c r="G11">
+        <v>0.342857142</v>
+      </c>
       <c r="I11">
         <v>0.75730994152046704</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
         <v>0.119618302481688</v>
       </c>
+      <c r="G12">
+        <v>6.6666665999999902E-2</v>
+      </c>
       <c r="I12">
         <v>0.84424242424242402</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
         <v>1.1364745134021601</v>
       </c>
+      <c r="G13">
+        <v>0.247692308</v>
+      </c>
       <c r="I13">
         <v>0.86788617886178798</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
         <v>0.74875279344046397</v>
       </c>
+      <c r="G14">
+        <v>4.14285719999999E-2</v>
+      </c>
       <c r="I14">
         <v>0.85906862745098</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
         <v>0.16602481507187999</v>
       </c>
+      <c r="G15">
+        <v>0.47538461599999998</v>
+      </c>
       <c r="I15">
         <v>0.80872093023255798</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
         <v>1.13960505036602</v>
+      </c>
+      <c r="G16">
+        <v>0.54933333399999995</v>
       </c>
       <c r="I16">
         <v>0.86959064327485303</v>
@@ -13418,11 +14455,17 @@
       <c r="B17">
         <v>0</v>
       </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17">
         <v>0.55904790936231097</v>
+      </c>
+      <c r="G17">
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="I17">
         <v>0.81881533101045301</v>
@@ -13435,11 +14478,17 @@
       <c r="B18">
         <v>0</v>
       </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
         <v>0.13247386743502201</v>
+      </c>
+      <c r="G18">
+        <v>0.42399999999999999</v>
       </c>
       <c r="I18">
         <v>0.85608747044917199</v>
@@ -13452,11 +14501,17 @@
       <c r="B19">
         <v>0</v>
       </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="F19">
         <v>0.30660298919399198</v>
+      </c>
+      <c r="G19">
+        <v>0.347142858</v>
       </c>
       <c r="I19">
         <v>0.84061771561771503</v>
@@ -13469,11 +14524,17 @@
       <c r="B20">
         <v>0</v>
       </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
         <v>0.67594341076745601</v>
+      </c>
+      <c r="G20">
+        <v>0.61833333399999901</v>
       </c>
       <c r="I20">
         <v>0.83110465116278998</v>
@@ -13486,11 +14547,17 @@
       <c r="B21">
         <v>0</v>
       </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
       <c r="E21">
         <v>1</v>
       </c>
       <c r="F21">
         <v>0.59163161136336595</v>
+      </c>
+      <c r="G21">
+        <v>0.34153846199999999</v>
       </c>
       <c r="I21">
         <v>0.88631022326674502</v>
@@ -13503,11 +14570,17 @@
       <c r="B22">
         <v>0</v>
       </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22">
         <v>0.56038052846741504</v>
+      </c>
+      <c r="G22">
+        <v>0.37066666599999898</v>
       </c>
       <c r="I22">
         <v>0.860744297719087</v>
@@ -13520,11 +14593,17 @@
       <c r="B23">
         <v>0</v>
       </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
         <v>0.90491976603661095</v>
+      </c>
+      <c r="G23">
+        <v>0.107999999999999</v>
       </c>
       <c r="I23">
         <v>0.79447674418604597</v>
@@ -13537,11 +14616,17 @@
       <c r="B24">
         <v>0</v>
       </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
         <v>0.33280813725629399</v>
+      </c>
+      <c r="G24">
+        <v>0.62714285800000003</v>
       </c>
       <c r="I24">
         <v>0.79447674418604597</v>
@@ -13554,11 +14639,17 @@
       <c r="B25">
         <v>0</v>
       </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
         <v>1.01020086064096</v>
+      </c>
+      <c r="G25">
+        <v>0.55333333399999896</v>
       </c>
       <c r="I25">
         <v>0.833720930232558</v>
@@ -13571,11 +14662,17 @@
       <c r="B26">
         <v>0</v>
       </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
         <v>0.171506233354456</v>
+      </c>
+      <c r="G26">
+        <v>0.37230769199999902</v>
       </c>
       <c r="I26">
         <v>0.85523255813953403</v>
@@ -13588,11 +14685,17 @@
       <c r="B27">
         <v>0</v>
       </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
         <v>0.56597043708066297</v>
+      </c>
+      <c r="G27">
+        <v>0.104</v>
       </c>
       <c r="I27">
         <v>0.768421052631579</v>
@@ -13605,11 +14708,17 @@
       <c r="B28">
         <v>0</v>
       </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
         <v>0.61487357655317898</v>
+      </c>
+      <c r="G28">
+        <v>0.24153846200000001</v>
       </c>
       <c r="I28">
         <v>0.88711583924349802</v>
@@ -13622,11 +14731,17 @@
       <c r="B29">
         <v>0</v>
       </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
         <v>2.4939859970258501E-3</v>
+      </c>
+      <c r="G29">
+        <v>0.31733333399999902</v>
       </c>
       <c r="I29">
         <v>0.80749128919860602</v>
@@ -13639,11 +14754,17 @@
       <c r="B30">
         <v>0</v>
       </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
         <v>0.17072700610625099</v>
+      </c>
+      <c r="G30">
+        <v>0.59599999999999997</v>
       </c>
       <c r="I30">
         <v>0.85454545454545405</v>
@@ -13656,11 +14777,17 @@
       <c r="B31">
         <v>0</v>
       </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
         <v>5.5839961386977201E-2</v>
+      </c>
+      <c r="G31">
+        <v>0.62142857200000001</v>
       </c>
       <c r="I31">
         <v>0.80784883720930201</v>
@@ -13673,11 +14800,17 @@
       <c r="B32">
         <v>0</v>
       </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
         <v>0.533418961196376</v>
+      </c>
+      <c r="G32">
+        <v>0.157142858</v>
       </c>
       <c r="I32">
         <v>0.84098837209302302</v>
@@ -13690,11 +14823,17 @@
       <c r="B33">
         <v>0</v>
       </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
         <v>0.129312601183009</v>
+      </c>
+      <c r="G33">
+        <v>0.34399999999999997</v>
       </c>
       <c r="I33">
         <v>0.87808460634547503</v>
@@ -13707,11 +14846,17 @@
       <c r="B34">
         <v>0</v>
       </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
         <v>7.4989811272123605E-2</v>
+      </c>
+      <c r="G34">
+        <v>0.54533333399999995</v>
       </c>
       <c r="I34">
         <v>0.82939393939393902</v>
@@ -13724,11 +14869,17 @@
       <c r="B35">
         <v>0</v>
       </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35">
         <v>0.11208697956019401</v>
+      </c>
+      <c r="G35">
+        <v>0.62142857200000001</v>
       </c>
       <c r="I35">
         <v>0.86754385964912195</v>
@@ -13741,11 +14892,17 @@
       <c r="B36">
         <v>0</v>
       </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
         <v>8.9371791849537197E-2</v>
+      </c>
+      <c r="G36">
+        <v>0.53857142799999902</v>
       </c>
       <c r="I36">
         <v>0.82373678025851904</v>
@@ -13758,11 +14915,17 @@
       <c r="B37">
         <v>0</v>
       </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37">
         <v>0.71255669863228899</v>
+      </c>
+      <c r="G37">
+        <v>0.49333333399999901</v>
       </c>
       <c r="I37">
         <v>0.768421052631579</v>
@@ -13775,11 +14938,17 @@
       <c r="B38">
         <v>0</v>
       </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38">
         <v>0.43578532471515702</v>
+      </c>
+      <c r="G38">
+        <v>0.133333334</v>
       </c>
       <c r="I38">
         <v>0.84243176178659995</v>
@@ -13792,11 +14961,17 @@
       <c r="B39">
         <v>0</v>
       </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
       <c r="E39">
         <v>0</v>
       </c>
       <c r="F39">
         <v>3.9966272436545498E-2</v>
+      </c>
+      <c r="G39">
+        <v>0.40142857199999998</v>
       </c>
       <c r="I39">
         <v>0.84207459207459201</v>
@@ -13809,11 +14984,17 @@
       <c r="B40">
         <v>0</v>
       </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
         <v>0.828501609830949</v>
+      </c>
+      <c r="G40">
+        <v>0.55733333399999996</v>
       </c>
       <c r="I40">
         <v>0.78281068524970898</v>
@@ -13826,11 +15007,17 @@
       <c r="B41">
         <v>0</v>
       </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41">
         <v>1.69942257238894</v>
+      </c>
+      <c r="G41">
+        <v>0.42307692400000002</v>
       </c>
       <c r="I41">
         <v>0.892732558139534</v>
@@ -13843,11 +15030,17 @@
       <c r="B42">
         <v>0</v>
       </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
       <c r="E42">
         <v>0</v>
       </c>
       <c r="F42">
         <v>1.3882414331950801</v>
+      </c>
+      <c r="G42">
+        <v>0.15428571399999899</v>
       </c>
       <c r="I42">
         <v>0.82971464019851104</v>
@@ -13860,11 +15053,17 @@
       <c r="B43">
         <v>1</v>
       </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
       <c r="E43">
         <v>1</v>
       </c>
       <c r="F43">
         <v>0.37330950232354698</v>
+      </c>
+      <c r="G43">
+        <v>0.44571428599999902</v>
       </c>
       <c r="I43">
         <v>0.80807200929152101</v>
@@ -13877,11 +15076,17 @@
       <c r="B44">
         <v>1</v>
       </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="F44">
         <v>1.3298808907840201</v>
+      </c>
+      <c r="G44">
+        <v>0.375384616</v>
       </c>
       <c r="I44">
         <v>0.84869976359337995</v>
@@ -13894,11 +15099,17 @@
       <c r="B45">
         <v>1</v>
       </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="F45">
         <v>0.89985930724313201</v>
+      </c>
+      <c r="G45">
+        <v>0.59285714199999995</v>
       </c>
       <c r="I45">
         <v>0.91462703962703895</v>
@@ -13911,11 +15122,17 @@
       <c r="B46">
         <v>1</v>
       </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
       <c r="E46">
         <v>1</v>
       </c>
       <c r="F46">
         <v>0.39613436244925199</v>
+      </c>
+      <c r="G46">
+        <v>0.39571428599999903</v>
       </c>
       <c r="I46">
         <v>0.86511627906976696</v>
@@ -13928,11 +15145,17 @@
       <c r="B47">
         <v>1</v>
       </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
       <c r="E47">
         <v>1</v>
       </c>
       <c r="F47">
         <v>5.0830754786535795E-4</v>
+      </c>
+      <c r="G47">
+        <v>0.56666666600000004</v>
       </c>
       <c r="I47">
         <v>0.88976608187134498</v>
@@ -13945,11 +15168,17 @@
       <c r="B48">
         <v>1</v>
       </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48">
         <v>0.162271350450124</v>
+      </c>
+      <c r="G48">
+        <v>0.29428571399999998</v>
       </c>
       <c r="I48">
         <v>0.89198606271777003</v>
@@ -13962,11 +15191,17 @@
       <c r="B49">
         <v>1</v>
       </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49">
         <v>0.33274397359477398</v>
+      </c>
+      <c r="G49">
+        <v>0.14000000000000001</v>
       </c>
       <c r="I49">
         <v>0.896886016451233</v>
@@ -13979,11 +15214,17 @@
       <c r="B50">
         <v>1</v>
       </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
       <c r="E50">
         <v>1</v>
       </c>
       <c r="F50">
         <v>8.9740799961524495E-2</v>
+      </c>
+      <c r="G50">
+        <v>0.60666666599999997</v>
       </c>
       <c r="I50">
         <v>0.91521486643437799</v>
@@ -13996,11 +15237,17 @@
       <c r="B51">
         <v>1</v>
       </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
       <c r="E51">
         <v>1</v>
       </c>
       <c r="F51">
         <v>7.2728178914915802E-3</v>
+      </c>
+      <c r="G51">
+        <v>0.18266666599999901</v>
       </c>
       <c r="I51">
         <v>0.80436046511627901</v>
@@ -14013,11 +15260,17 @@
       <c r="B52">
         <v>1</v>
       </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
       <c r="E52">
         <v>1</v>
       </c>
       <c r="F52">
         <v>0.60007602096368096</v>
+      </c>
+      <c r="G52">
+        <v>2.9333333999999898E-2</v>
       </c>
       <c r="I52">
         <v>0.74679487179487103</v>
@@ -14030,11 +15283,17 @@
       <c r="B53">
         <v>1</v>
       </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
       <c r="E53">
         <v>1</v>
       </c>
       <c r="F53">
         <v>0.65940872444911702</v>
+      </c>
+      <c r="G53">
+        <v>0.39714285799999999</v>
       </c>
       <c r="I53">
         <v>0.90348837209302302</v>
@@ -14047,11 +15306,17 @@
       <c r="B54">
         <v>1</v>
       </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
       <c r="E54">
         <v>1</v>
       </c>
       <c r="F54">
         <v>0.13121850827572301</v>
+      </c>
+      <c r="G54">
+        <v>0.62428571399999999</v>
       </c>
       <c r="I54">
         <v>0.89140534262485405</v>
@@ -14064,11 +15329,17 @@
       <c r="B55">
         <v>1</v>
       </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
       <c r="E55">
         <v>1</v>
       </c>
       <c r="F55">
         <v>0.26117819385752999</v>
+      </c>
+      <c r="G55">
+        <v>0.42249999999999999</v>
       </c>
       <c r="I55">
         <v>0.85348837209302297</v>
@@ -14081,11 +15352,17 @@
       <c r="B56">
         <v>1</v>
       </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="F56">
         <v>0.51873242164687705</v>
+      </c>
+      <c r="G56">
+        <v>2.1333333999999898E-2</v>
       </c>
       <c r="I56">
         <v>0.815988372093023</v>
@@ -14098,11 +15375,17 @@
       <c r="B57">
         <v>1</v>
       </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
       <c r="E57">
         <v>1</v>
       </c>
       <c r="F57">
         <v>1.4268971786037199</v>
+      </c>
+      <c r="G57">
+        <v>0.22</v>
       </c>
       <c r="I57">
         <v>0.84869976359337995</v>
@@ -14115,11 +15398,17 @@
       <c r="B58">
         <v>1</v>
       </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
       <c r="E58">
         <v>0</v>
       </c>
       <c r="F58">
         <v>0.483098107286622</v>
+      </c>
+      <c r="G58">
+        <v>0.16666666599999999</v>
       </c>
       <c r="I58">
         <v>0.86192714453583996</v>
@@ -14132,11 +15421,17 @@
       <c r="B59">
         <v>1</v>
       </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
       <c r="E59">
         <v>1</v>
       </c>
       <c r="F59">
         <v>0.49453111463043598</v>
+      </c>
+      <c r="G59">
+        <v>0.71599999999999997</v>
       </c>
       <c r="I59">
         <v>0.77953216374268997</v>
@@ -14149,11 +15444,17 @@
       <c r="B60">
         <v>1</v>
       </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
       <c r="E60">
         <v>1</v>
       </c>
       <c r="F60">
         <v>0.25659752724507401</v>
+      </c>
+      <c r="G60">
+        <v>0.28923077000000003</v>
       </c>
       <c r="I60">
         <v>0.87648809523809501</v>
@@ -14166,11 +15467,17 @@
       <c r="B61">
         <v>1</v>
       </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
       <c r="E61">
         <v>1</v>
       </c>
       <c r="F61">
         <v>0.15141241270105199</v>
+      </c>
+      <c r="G61">
+        <v>4.6153839999999403E-3</v>
       </c>
       <c r="I61">
         <v>0.90246768507637998</v>
@@ -14183,11 +15490,17 @@
       <c r="B62">
         <v>1</v>
       </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
       <c r="E62">
         <v>1</v>
       </c>
       <c r="F62">
         <v>0.25494998774777999</v>
+      </c>
+      <c r="G62">
+        <v>0.70799999999999996</v>
       </c>
       <c r="I62">
         <v>0.87865497076023302</v>
@@ -14200,11 +15513,17 @@
       <c r="B63">
         <v>1</v>
       </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
       <c r="E63">
         <v>1</v>
       </c>
       <c r="F63">
         <v>1.77540067705024</v>
+      </c>
+      <c r="G63">
+        <v>0.08</v>
       </c>
       <c r="I63">
         <v>0.78310104529616698</v>
@@ -14217,11 +15536,17 @@
       <c r="B64">
         <v>1</v>
       </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
       <c r="E64">
         <v>0</v>
       </c>
       <c r="F64">
         <v>0.62284723611592996</v>
+      </c>
+      <c r="G64">
+        <v>0.20533333400000001</v>
       </c>
       <c r="I64">
         <v>0.90174418604651096</v>
@@ -14234,11 +15559,17 @@
       <c r="B65">
         <v>1</v>
       </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
       <c r="E65">
         <v>1</v>
       </c>
       <c r="F65">
         <v>0.261608356926185</v>
+      </c>
+      <c r="G65">
+        <v>0.342857142</v>
       </c>
       <c r="I65">
         <v>0.82373678025851904</v>
@@ -14251,11 +15582,17 @@
       <c r="B66">
         <v>1</v>
       </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
       <c r="E66">
         <v>1</v>
       </c>
       <c r="F66">
         <v>0.93572056974704398</v>
+      </c>
+      <c r="G66">
+        <v>0.27428571399999901</v>
       </c>
       <c r="I66">
         <v>0.80584795321637404</v>
@@ -14268,11 +15605,17 @@
       <c r="B67">
         <v>1</v>
       </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
       <c r="E67">
         <v>1</v>
       </c>
       <c r="F67">
         <v>5.8887059080366899E-2</v>
+      </c>
+      <c r="G67">
+        <v>0.65428571400000002</v>
       </c>
       <c r="I67">
         <v>0.79935370152761398</v>
@@ -14285,11 +15628,17 @@
       <c r="B68">
         <v>1</v>
       </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
       <c r="E68">
         <v>1</v>
       </c>
       <c r="F68">
         <v>0.13100705600314999</v>
+      </c>
+      <c r="G68">
+        <v>0.51200000000000001</v>
       </c>
       <c r="I68">
         <v>0.86754385964912195</v>
@@ -14302,11 +15651,17 @@
       <c r="B69">
         <v>1</v>
       </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
       <c r="E69">
         <v>1</v>
       </c>
       <c r="F69">
         <v>0.63460697626263696</v>
+      </c>
+      <c r="G69">
+        <v>0.22769230800000001</v>
       </c>
       <c r="I69">
         <v>0.83159117305458696</v>
@@ -14319,11 +15674,17 @@
       <c r="B70">
         <v>1</v>
       </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
       <c r="E70">
         <v>1</v>
       </c>
       <c r="F70">
         <v>0.98378128586267199</v>
+      </c>
+      <c r="G70">
+        <v>0.57428571399999995</v>
       </c>
       <c r="I70">
         <v>0.83894799054373503</v>
@@ -14336,11 +15697,17 @@
       <c r="B71">
         <v>1</v>
       </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
       <c r="E71">
         <v>1</v>
       </c>
       <c r="F71">
         <v>2.88395540532695E-2</v>
+      </c>
+      <c r="G71">
+        <v>0.745714286</v>
       </c>
       <c r="I71">
         <v>0.89481351981351898</v>
@@ -14353,11 +15720,17 @@
       <c r="B72">
         <v>1</v>
       </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
       <c r="E72">
         <v>1</v>
       </c>
       <c r="F72">
         <v>0.13394540758248</v>
+      </c>
+      <c r="G72">
+        <v>0.14000000000000001</v>
       </c>
       <c r="I72">
         <v>0.84360465116279004</v>
@@ -14370,11 +15743,17 @@
       <c r="B73">
         <v>1</v>
       </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
       <c r="E73">
         <v>1</v>
       </c>
       <c r="F73">
         <v>0.50248955698933595</v>
+      </c>
+      <c r="G73">
+        <v>0.42266666600000002</v>
       </c>
       <c r="I73">
         <v>0.90697674418604601</v>
@@ -14387,11 +15766,17 @@
       <c r="B74">
         <v>1</v>
       </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
       <c r="E74">
         <v>1</v>
       </c>
       <c r="F74">
         <v>0.64555887812979795</v>
+      </c>
+      <c r="G74">
+        <v>0.30249999999999999</v>
       </c>
       <c r="I74">
         <v>0.91056422569027595</v>
@@ -14404,11 +15789,17 @@
       <c r="B75">
         <v>1</v>
       </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
       <c r="E75">
         <v>1</v>
       </c>
       <c r="F75">
         <v>0.33069085435310303</v>
+      </c>
+      <c r="G75">
+        <v>0.06</v>
       </c>
       <c r="I75">
         <v>0.86985898942420603</v>
@@ -14421,11 +15812,17 @@
       <c r="B76">
         <v>1</v>
       </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
       <c r="E76">
         <v>1</v>
       </c>
       <c r="F76">
         <v>1.6753083362875401</v>
+      </c>
+      <c r="G76">
+        <v>4.8571428E-2</v>
       </c>
       <c r="I76">
         <v>0.80523255813953398</v>
@@ -14438,11 +15835,17 @@
       <c r="B77">
         <v>1</v>
       </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
       <c r="E77">
         <v>1</v>
       </c>
       <c r="F77">
         <v>0.62579730405548595</v>
+      </c>
+      <c r="G77">
+        <v>0.27</v>
       </c>
       <c r="I77">
         <v>0.89982373678025795</v>
@@ -14455,11 +15858,17 @@
       <c r="B78">
         <v>1</v>
       </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
       <c r="E78">
         <v>1</v>
       </c>
       <c r="F78">
         <v>0.46842218267706398</v>
+      </c>
+      <c r="G78">
+        <v>0.13866666599999999</v>
       </c>
       <c r="I78">
         <v>0.78154761904761905</v>
@@ -14472,11 +15881,17 @@
       <c r="B79">
         <v>1</v>
       </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
       <c r="E79">
         <v>1</v>
       </c>
       <c r="F79">
         <v>0.59209443934954897</v>
+      </c>
+      <c r="G79">
+        <v>0.152307691999999</v>
       </c>
       <c r="I79">
         <v>0.84122807017543799</v>
@@ -14489,11 +15904,17 @@
       <c r="B80">
         <v>1</v>
       </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
       <c r="E80">
         <v>1</v>
       </c>
       <c r="F80">
         <v>0.79708789444466499</v>
+      </c>
+      <c r="G80">
+        <v>0.13285714200000001</v>
       </c>
       <c r="I80">
         <v>0.83490011750881299</v>
@@ -14506,11 +15927,17 @@
       <c r="B81">
         <v>1</v>
       </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
       <c r="E81">
         <v>0</v>
       </c>
       <c r="F81">
         <v>0.35870713750562</v>
+      </c>
+      <c r="G81">
+        <v>0.48285714200000002</v>
       </c>
       <c r="I81">
         <v>0.74825174825174801</v>
@@ -14523,11 +15950,17 @@
       <c r="B82">
         <v>1</v>
       </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
       <c r="E82">
         <v>1</v>
       </c>
       <c r="F82">
         <v>0.44077515986564197</v>
+      </c>
+      <c r="G82">
+        <v>0.118666666</v>
       </c>
       <c r="I82">
         <v>0.75987224157955802</v>
@@ -14540,11 +15973,17 @@
       <c r="B83">
         <v>1</v>
       </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
       <c r="E83">
         <v>1</v>
       </c>
       <c r="F83">
         <v>0.57011991729475198</v>
+      </c>
+      <c r="G83">
+        <v>5.5999999999999897E-2</v>
       </c>
       <c r="I83">
         <v>0.79878787878787805</v>
@@ -14557,11 +15996,17 @@
       <c r="B84">
         <v>1</v>
       </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
       <c r="E84">
         <v>0</v>
       </c>
       <c r="F84">
         <v>0.32246658767414399</v>
+      </c>
+      <c r="G84">
+        <v>0.21714285799999999</v>
       </c>
       <c r="I84">
         <v>0.86549707602339099</v>
@@ -19159,10 +20604,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29B8CFE-CE27-48D0-99D6-D06E8FAF20D9}">
-  <dimension ref="A1:J1001"/>
+  <dimension ref="A1:P1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C84"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19177,9 +20622,11 @@
     <col min="8" max="8" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -19187,25 +20634,37 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="F1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="G1" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -19228,16 +20687,31 @@
         <v>0.462857142</v>
       </c>
       <c r="H2" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="I2">
         <v>0.88023255813953405</v>
       </c>
       <c r="J2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="L2" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2">
+        <v>0.66265060240963802</v>
+      </c>
+      <c r="N2">
+        <v>0.69047619047619002</v>
+      </c>
+      <c r="O2">
+        <v>0.36585365853658502</v>
+      </c>
+      <c r="P2">
+        <v>0.78281068524970898</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -19263,10 +20737,25 @@
         <v>0.88303571428571404</v>
       </c>
       <c r="J3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="L3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M3">
+        <v>0.80722891566264998</v>
+      </c>
+      <c r="N3">
+        <v>0.69047619047619002</v>
+      </c>
+      <c r="O3">
+        <v>7.3170731707316999E-2</v>
+      </c>
+      <c r="P3">
+        <v>0.808652729384436</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -19294,8 +20783,23 @@
       <c r="J4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>100</v>
+      </c>
+      <c r="M4">
+        <v>0.86746987951807197</v>
+      </c>
+      <c r="N4">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="O4">
+        <v>9.7560975609756101E-2</v>
+      </c>
+      <c r="P4">
+        <v>0.87166085946573701</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -19321,7 +20825,7 @@
         <v>0.89883040935672498</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -19347,7 +20851,7 @@
         <v>0.86507444168734404</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -19373,7 +20877,7 @@
         <v>0.89732142857142805</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -19399,7 +20903,7 @@
         <v>0.82053571428571404</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -19425,7 +20929,7 @@
         <v>0.95087209302325504</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -19451,7 +20955,7 @@
         <v>0.915116279069767</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -19477,7 +20981,7 @@
         <v>0.87865497076023302</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -19503,7 +21007,7 @@
         <v>0.82393939393939397</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -19529,7 +21033,7 @@
         <v>0.83246225319395994</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -19555,7 +21059,7 @@
         <v>0.88633578431372495</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -19581,7 +21085,7 @@
         <v>0.89098837209302295</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Adds grad cam visualizations. Creates some figures and amends the report.
</commit_message>
<xml_diff>
--- a/Solution3/Results/Bootstrapping Results.xlsx
+++ b/Solution3/Results/Bootstrapping Results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BDB9C3-8420-471F-BB15-1C07FF50A1F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE78D9F-20F1-49F1-B591-D2E69BDB30C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,17 +13,23 @@
     <sheet name="NoCrop Facing Same Dir" sheetId="2" r:id="rId3"/>
     <sheet name="Cropped Facing Same Dir" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="115">
   <si>
     <t>Image</t>
   </si>
@@ -366,6 +372,9 @@
   <si>
     <t>95% CI 0.6477541371158393 to 0.8589285714285714</t>
   </si>
+  <si>
+    <t>AUC stdev</t>
+  </si>
 </sst>
 </file>
 
@@ -407,7 +416,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,13 +450,34 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -457,7 +487,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -465,6 +495,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -748,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P1001"/>
+  <dimension ref="A1:Q1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,10 +802,10 @@
     <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -797,20 +830,24 @@
       <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -838,23 +875,24 @@
       <c r="J2" t="s">
         <v>110</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="8">
         <v>0.56626506024096301</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="8">
         <v>0.57142857142857095</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="8">
         <v>0.439024390243902</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="8">
         <v>0.63066202090592305</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="8"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -879,23 +917,24 @@
       <c r="J3" t="s">
         <v>112</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="8">
         <v>0.80722891566264998</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="8">
         <v>0.69047619047619002</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="8">
         <v>7.3170731707316999E-2</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="8">
         <v>0.808652729384436</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -920,23 +959,26 @@
       <c r="J4" t="s">
         <v>113</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="8">
         <v>0.74698795180722799</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="8">
         <v>0.73809523809523803</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="8">
         <v>0.24390243902438999</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="8">
         <v>0.76829268292682895</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="8">
+        <v>5.3877155917426298E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -959,7 +1001,7 @@
         <v>0.69356725146198805</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -982,7 +1024,7 @@
         <v>0.70099255583126496</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1005,7 +1047,7 @@
         <v>0.746428571428571</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1028,7 +1070,7 @@
         <v>0.75684523809523796</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1051,7 +1093,7 @@
         <v>0.85436046511627906</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1074,7 +1116,7 @@
         <v>0.74796511627906903</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1097,7 +1139,7 @@
         <v>0.56725146198830401</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1120,7 +1162,7 @@
         <v>0.72363636363636297</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1143,7 +1185,7 @@
         <v>0.79529616724738605</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1166,7 +1208,7 @@
         <v>0.73774509803921495</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1189,7 +1231,7 @@
         <v>0.65145348837209305</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -7368,10 +7410,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC718A7F-4416-4837-9CBF-C11F5F01DF1B}">
-  <dimension ref="A1:P1001"/>
+  <dimension ref="A1:Q1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7387,10 +7429,10 @@
     <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7415,20 +7457,24 @@
       <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -7456,23 +7502,24 @@
       <c r="J2" t="s">
         <v>107</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="8">
         <v>0.65060240963855398</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="8">
         <v>0.69047619047619002</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="8">
         <v>0.39024390243902402</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="8">
         <v>0.70789779326364699</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="8"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -7497,23 +7544,24 @@
       <c r="J3" t="s">
         <v>108</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="8">
         <v>0.80722891566264998</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="8">
         <v>0.69047619047619002</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="8">
         <v>7.3170731707316999E-2</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="8">
         <v>0.808652729384436</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -7538,23 +7586,26 @@
       <c r="J4" t="s">
         <v>109</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="8">
         <v>0.843373493975903</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="8">
         <v>0.80952380952380898</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="8">
         <v>0.12195121951219499</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="8">
         <v>0.81765389082462203</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="8">
+        <v>5.0994750714691901E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -7577,7 +7628,7 @@
         <v>0.76637426900584704</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -7600,7 +7651,7 @@
         <v>0.83281637717121504</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -7623,7 +7674,7 @@
         <v>0.85446428571428501</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -7646,7 +7697,7 @@
         <v>0.81785714285714195</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -7669,7 +7720,7 @@
         <v>0.90436046511627899</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -7692,7 +7743,7 @@
         <v>0.892732558139534</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -7715,7 +7766,7 @@
         <v>0.73713450292397598</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -7738,7 +7789,7 @@
         <v>0.83393939393939298</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -7761,7 +7812,7 @@
         <v>0.85598141695702601</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -7784,7 +7835,7 @@
         <v>0.82965686274509798</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -7807,7 +7858,7 @@
         <v>0.80872093023255798</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -13986,10 +14037,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD840D1-1D4B-4BA9-B0B8-24F9FD7C2C86}">
-  <dimension ref="A1:P1001"/>
+  <dimension ref="A1:Q1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14005,10 +14056,10 @@
     <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14033,20 +14084,24 @@
       <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -14074,23 +14129,24 @@
       <c r="J2" t="s">
         <v>102</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="8">
         <v>0.67469879518072196</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="8">
         <v>0.64285714285714202</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="8">
         <v>0.292682926829268</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="8">
         <v>0.77061556329849001</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="8"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -14115,23 +14171,24 @@
       <c r="J3" t="s">
         <v>103</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="8">
         <v>0.80722891566264998</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="8">
         <v>0.69047619047619002</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="8">
         <v>7.3170731707316999E-2</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="8">
         <v>0.808652729384436</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -14156,23 +14213,26 @@
       <c r="J4" t="s">
         <v>104</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="8">
         <v>0.843373493975903</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="8">
         <v>0.83333333333333304</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="8">
         <v>0.146341463414634</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="8">
         <v>0.88385598141695698</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="8">
+        <v>3.6599413704818999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -14195,7 +14255,7 @@
         <v>0.85029239766081799</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -14218,7 +14278,7 @@
         <v>0.86507444168734404</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -14241,7 +14301,7 @@
         <v>0.81279761904761905</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -14264,7 +14324,7 @@
         <v>0.80625000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -14287,7 +14347,7 @@
         <v>0.878488372093023</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -14310,7 +14370,7 @@
         <v>0.82936046511627903</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -14333,7 +14393,7 @@
         <v>0.75730994152046704</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -14356,7 +14416,7 @@
         <v>0.84424242424242402</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -14379,7 +14439,7 @@
         <v>0.86788617886178798</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -14402,7 +14462,7 @@
         <v>0.85906862745098</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -14425,7 +14485,7 @@
         <v>0.80872093023255798</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -20604,10 +20664,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29B8CFE-CE27-48D0-99D6-D06E8FAF20D9}">
-  <dimension ref="A1:P1001"/>
+  <dimension ref="A1:Q1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20623,10 +20683,10 @@
     <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -20651,20 +20711,24 @@
       <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" t="s">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -20695,23 +20759,24 @@
       <c r="J2" t="s">
         <v>98</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="8">
         <v>0.66265060240963802</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="8">
         <v>0.69047619047619002</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="8">
         <v>0.36585365853658502</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="8">
         <v>0.78281068524970898</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="8"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -20739,23 +20804,24 @@
       <c r="J3" t="s">
         <v>97</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="8">
         <v>0.80722891566264998</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="8">
         <v>0.69047619047619002</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="8">
         <v>7.3170731707316999E-2</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="8">
         <v>0.808652729384436</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -20783,23 +20849,26 @@
       <c r="J4" t="s">
         <v>99</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="8">
         <v>0.86746987951807197</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="8">
         <v>0.83333333333333304</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="8">
         <v>9.7560975609756101E-2</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="8">
         <v>0.87166085946573701</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4" s="8">
+        <v>4.2669754473986202E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -20825,7 +20894,7 @@
         <v>0.89883040935672498</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -20851,7 +20920,7 @@
         <v>0.86507444168734404</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -20877,7 +20946,7 @@
         <v>0.89732142857142805</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -20903,7 +20972,7 @@
         <v>0.82053571428571404</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -20929,7 +20998,7 @@
         <v>0.95087209302325504</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -20955,7 +21024,7 @@
         <v>0.915116279069767</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -20981,7 +21050,7 @@
         <v>0.87865497076023302</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -21007,7 +21076,7 @@
         <v>0.82393939393939397</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -21033,7 +21102,7 @@
         <v>0.83246225319395994</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -21059,7 +21128,7 @@
         <v>0.88633578431372495</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -21085,7 +21154,7 @@
         <v>0.89098837209302295</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -21840,19 +21909,19 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45">
+      <c r="B45" s="9">
+        <v>1</v>
+      </c>
+      <c r="C45" s="9">
+        <v>0</v>
+      </c>
+      <c r="D45" s="9">
+        <v>1</v>
+      </c>
+      <c r="E45" s="9">
         <v>0</v>
       </c>
       <c r="F45">
@@ -22895,6 +22964,14 @@
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <f>PEARSON(C2:C84,D2:D84)</f>
+        <v>0.20018249050098397</v>
+      </c>
+      <c r="F88">
+        <f>PEARSON(F2:F84,G2:G84)</f>
+        <v>-9.3013591528384107E-2</v>
+      </c>
       <c r="I88">
         <v>0.89169570267131204</v>
       </c>
@@ -27466,5 +27543,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixes inceptionv4 features and LGBM uses. Adds new results
</commit_message>
<xml_diff>
--- a/Solution3/Results/Bootstrapping Results.xlsx
+++ b/Solution3/Results/Bootstrapping Results.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71788E19-F7A3-4088-A7F5-B5D263761019}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A934EF3-1659-41B4-81F1-AC207BD0D1B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NoCrop Original" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,8 @@
     <sheet name="Cropped Facing Same Dir" sheetId="4" r:id="rId4"/>
     <sheet name="Cropped All MirrorRotations" sheetId="5" r:id="rId5"/>
     <sheet name="NoCrop All MirrorRotations" sheetId="6" r:id="rId6"/>
+    <sheet name="LGBM scores with Inceptionv4" sheetId="7" r:id="rId7"/>
+    <sheet name="LGBM scores with VGG19" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="140">
   <si>
     <t>Image</t>
   </si>
@@ -400,12 +402,63 @@
   <si>
     <t>Machine+Radiologist+PCA(83)</t>
   </si>
+  <si>
+    <t>Machine(No crop)</t>
+  </si>
+  <si>
+    <t>Machine+Radiologist(No crop)</t>
+  </si>
+  <si>
+    <t>Machine(No crop same dir)</t>
+  </si>
+  <si>
+    <t>Machine+Radiologist(No crop same dir)</t>
+  </si>
+  <si>
+    <t>Machine(Crop)</t>
+  </si>
+  <si>
+    <t>Machine+Radiologist(Crop)</t>
+  </si>
+  <si>
+    <t>Machine(Crop same dir)</t>
+  </si>
+  <si>
+    <t>Machine+Radiologist(Crop same dir)</t>
+  </si>
+  <si>
+    <t>95% CI</t>
+  </si>
+  <si>
+    <t>0.7988372093023256 to 0.9415204678362573</t>
+  </si>
+  <si>
+    <t>0.7096969696969697 to 0.8866279069767442</t>
+  </si>
+  <si>
+    <t>0.7377906976744186 to 0.9065040650406504</t>
+  </si>
+  <si>
+    <t>0.6812443727490995 to 0.872610294117647</t>
+  </si>
+  <si>
+    <t>0.6154761904761905 to 0.8273255813953488</t>
+  </si>
+  <si>
+    <t>0.6554373522458629 to 0.8531139835487662</t>
+  </si>
+  <si>
+    <t>0.6958333333333333 to 0.8854166666666667</t>
+  </si>
+  <si>
+    <t>0.6321138211382114 to 0.8378378378378378</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,6 +489,23 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -512,7 +582,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -527,6 +597,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -27580,7 +27655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A75A154C-2D9E-4795-A2A3-25ACAD2037BE}">
   <dimension ref="A1:Q1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
@@ -34488,7 +34563,7 @@
   <dimension ref="A1:Q1001"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="L1" sqref="L1:Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41388,4 +41463,461 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7316FA4A-6216-460C-BD03-91A9D3AC2A27}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.80722891566264998</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.69047619047619002</v>
+      </c>
+      <c r="D2" s="8">
+        <v>7.3170731707316999E-2</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.808652729384436</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0.686746987951807</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.34146341463414598</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.74332171893147503</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="15">
+        <v>0.78313253012048101</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0.80952380952380898</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0.24390243902438999</v>
+      </c>
+      <c r="E4" s="18">
+        <v>0.87804878048780499</v>
+      </c>
+      <c r="F4" s="15">
+        <v>3.5909827402117803E-2</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0.61445783132530096</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.439024390243902</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.68118466898954699</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0.686746987951807</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.69047619047619002</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.31707317073170699</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.80487804878048697</v>
+      </c>
+      <c r="F6" s="8">
+        <v>4.7384989128586602E-2</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0.56626506024096301</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.69047619047619002</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.56097560975609695</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.62485481997677095</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0.67469879518072196</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.76190476190476097</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.41463414634146301</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.787456445993031</v>
+      </c>
+      <c r="F8" s="8">
+        <v>4.82837220275769E-2</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9">
+        <v>0.62650602409638501</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.69047619047619002</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.439024390243902</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.67595818815330999</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0.73493975903614395</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.76190476190476097</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.292682926829268</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.82810685249709604</v>
+      </c>
+      <c r="F10" s="8">
+        <v>4.1748983608351803E-2</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF770C3B-E22F-4DB6-8CD6-57FAF4235673}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.80722891566264998</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.69047619047619002</v>
+      </c>
+      <c r="D2" s="8">
+        <v>7.3170731707316999E-2</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.808652729384436</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0.53012048192771</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.54761904761904701</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.48780487804877998</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.55400696864111498</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="17">
+        <v>0.62650602409638501</v>
+      </c>
+      <c r="C4" s="17">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="D4" s="17">
+        <v>0.41463414634146301</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0.73983739837398299</v>
+      </c>
+      <c r="F4" s="17">
+        <v>5.2181565830162702E-2</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0.63855421686746905</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.76190476190476097</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.48780487804877998</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.65853658536585302</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0.74698795180722799</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.85714285714285698</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.36585365853658502</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.80139372822299604</v>
+      </c>
+      <c r="F6" s="8">
+        <v>4.8627638823700997E-2</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0.53012048192771</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.59523809523809501</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.53658536585365801</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.51567944250871001</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0.63855421686746905</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.39024390243902402</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.72415795586527298</v>
+      </c>
+      <c r="F8" s="8">
+        <v>5.425109027076E-2</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9">
+        <v>0.62650602409638501</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.61904761904761896</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.36585365853658502</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.64634146341463405</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0.66265060240963802</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.64285714285714202</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0.31707317073170699</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.76335656213704906</v>
+      </c>
+      <c r="F10" s="8">
+        <v>5.14714105723727E-2</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>